<commit_message>
Added routine to get suffixes for each melt prefix
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4669,8 +4669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:VC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="UT1" workbookViewId="0">
-      <selection activeCell="VF1" sqref="VF1:VF1048576"/>
+    <sheetView tabSelected="1" topLeftCell="UP1" workbookViewId="0">
+      <selection activeCell="SO1" sqref="SO1:VE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.88671875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6561,19 +6561,19 @@
       </c>
       <c r="ES2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU2" s="1" t="str">
         <f t="shared" ref="EU2:EV2" ca="1" si="0">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV2" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW2" t="s">
         <v>7</v>
@@ -6583,19 +6583,19 @@
       </c>
       <c r="GC2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE2" s="1" t="str">
         <f t="shared" ref="GE2:GF2" ca="1" si="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF2" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG2" t="s">
         <v>8</v>
@@ -6605,19 +6605,19 @@
       </c>
       <c r="HM2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO2" s="1" t="str">
         <f t="shared" ref="HO2:HP2" ca="1" si="2">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP2" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ2" t="s">
         <v>7</v>
@@ -6627,19 +6627,19 @@
       </c>
       <c r="IW2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY2" s="1" t="str">
         <f t="shared" ref="IY2:IZ2" ca="1" si="3">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ2" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA2" t="s">
         <v>7</v>
@@ -6649,19 +6649,19 @@
       </c>
       <c r="KG2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI2" s="1" t="str">
         <f t="shared" ref="KI2:KJ2" ca="1" si="4">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ2" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK2" t="s">
         <v>7</v>
@@ -6671,19 +6671,19 @@
       </c>
       <c r="LQ2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS2" s="1" t="str">
         <f t="shared" ref="LS2:LT2" ca="1" si="5">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT2" s="1" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU2" t="s">
         <v>7</v>
@@ -6693,19 +6693,19 @@
       </c>
       <c r="NA2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC2" s="1" t="str">
         <f t="shared" ref="NC2:ND2" ca="1" si="6">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND2" s="1" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE2" t="s">
         <v>7</v>
@@ -6715,19 +6715,19 @@
       </c>
       <c r="OK2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM2" s="1" t="str">
         <f t="shared" ref="OM2:ON2" ca="1" si="7">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON2" s="1" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO2" t="s">
         <v>7</v>
@@ -6737,19 +6737,19 @@
       </c>
       <c r="PU2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW2" s="1" t="str">
         <f t="shared" ref="PW2:PX2" ca="1" si="8">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX2" s="1" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY2" t="s">
         <v>7</v>
@@ -6798,19 +6798,19 @@
       </c>
       <c r="TY2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ2" s="1" t="str">
         <f ca="1">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA2" s="1" t="str">
         <f t="shared" ref="UA2:UB2" ca="1" si="9">CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)&amp;CHAR(RAND()*26+97)</f>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB2" s="1" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC2" t="s">
         <v>691</v>
@@ -7002,19 +7002,19 @@
       </c>
       <c r="ES3" t="str">
         <f ca="1">ES$2</f>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET3" t="str">
         <f t="shared" ref="ET3:EV3" ca="1" si="10">ET$2</f>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU3" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV3" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW3" t="s">
         <v>7</v>
@@ -7024,19 +7024,19 @@
       </c>
       <c r="GC3" t="str">
         <f ca="1">GC$2</f>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD3" t="str">
         <f t="shared" ref="GD3:GF3" ca="1" si="11">GD$2</f>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE3" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF3" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG3" t="s">
         <v>8</v>
@@ -7046,19 +7046,19 @@
       </c>
       <c r="HM3" t="str">
         <f ca="1">HM$2</f>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN3" t="str">
         <f t="shared" ref="HN3:HP3" ca="1" si="12">HN$2</f>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO3" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP3" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ3" t="s">
         <v>7</v>
@@ -7068,19 +7068,19 @@
       </c>
       <c r="IW3" t="str">
         <f ca="1">IW$2</f>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX3" t="str">
         <f t="shared" ref="IX3:IZ3" ca="1" si="13">IX$2</f>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY3" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ3" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA3" t="s">
         <v>7</v>
@@ -7090,19 +7090,19 @@
       </c>
       <c r="KG3" t="str">
         <f ca="1">KG$2</f>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH3" t="str">
         <f t="shared" ref="KH3:KJ3" ca="1" si="14">KH$2</f>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ3" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK3" t="s">
         <v>7</v>
@@ -7112,19 +7112,19 @@
       </c>
       <c r="LQ3" t="str">
         <f ca="1">LQ$2</f>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR3" t="str">
         <f t="shared" ref="LR3:LT3" ca="1" si="15">LR$2</f>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS3" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT3" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU3" t="s">
         <v>7</v>
@@ -7134,19 +7134,19 @@
       </c>
       <c r="NA3" t="str">
         <f ca="1">NA$2</f>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB3" t="str">
         <f t="shared" ref="NB3:ND3" ca="1" si="16">NB$2</f>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC3" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND3" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE3" t="s">
         <v>7</v>
@@ -7156,19 +7156,19 @@
       </c>
       <c r="OK3" t="str">
         <f ca="1">OK$2</f>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL3" t="str">
         <f t="shared" ref="OL3:ON3" ca="1" si="17">OL$2</f>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM3" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON3" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO3" t="s">
         <v>7</v>
@@ -7178,19 +7178,19 @@
       </c>
       <c r="PU3" t="str">
         <f ca="1">PU$2</f>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV3" t="str">
         <f t="shared" ref="PV3:PX3" ca="1" si="18">PV$2</f>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW3" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX3" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY3" t="s">
         <v>7</v>
@@ -7239,19 +7239,19 @@
       </c>
       <c r="TY3" t="str">
         <f ca="1">TY$2</f>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ3" t="str">
         <f t="shared" ref="TZ3:UB3" ca="1" si="19">TZ$2</f>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA3" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB3" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC3" t="s">
         <v>691</v>
@@ -7443,19 +7443,19 @@
       </c>
       <c r="ES4" t="str">
         <f t="shared" ref="ES4:EV10" ca="1" si="20">ES$2</f>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET4" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU4" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV4" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW4" t="s">
         <v>7</v>
@@ -7465,19 +7465,19 @@
       </c>
       <c r="GC4" t="str">
         <f t="shared" ref="GC4:GF10" ca="1" si="21">GC$2</f>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD4" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE4" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF4" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG4" t="s">
         <v>8</v>
@@ -7487,19 +7487,19 @@
       </c>
       <c r="HM4" t="str">
         <f t="shared" ref="HM4:HP10" ca="1" si="22">HM$2</f>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN4" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO4" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP4" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ4" t="s">
         <v>7</v>
@@ -7509,19 +7509,19 @@
       </c>
       <c r="IW4" t="str">
         <f t="shared" ref="IW4:IZ10" ca="1" si="23">IW$2</f>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA4" t="s">
         <v>7</v>
@@ -7531,19 +7531,19 @@
       </c>
       <c r="KG4" t="str">
         <f t="shared" ref="KG4:KJ10" ca="1" si="24">KG$2</f>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH4" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI4" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ4" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK4" t="s">
         <v>7</v>
@@ -7553,19 +7553,19 @@
       </c>
       <c r="LQ4" t="str">
         <f t="shared" ref="LQ4:LT10" ca="1" si="25">LQ$2</f>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR4" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS4" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT4" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU4" t="s">
         <v>7</v>
@@ -7575,19 +7575,19 @@
       </c>
       <c r="NA4" t="str">
         <f t="shared" ref="NA4:ND10" ca="1" si="26">NA$2</f>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB4" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC4" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND4" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE4" t="s">
         <v>7</v>
@@ -7597,19 +7597,19 @@
       </c>
       <c r="OK4" t="str">
         <f t="shared" ref="OK4:ON10" ca="1" si="27">OK$2</f>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL4" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM4" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON4" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO4" t="s">
         <v>7</v>
@@ -7619,19 +7619,19 @@
       </c>
       <c r="PU4" t="str">
         <f t="shared" ref="PU4:PX10" ca="1" si="28">PU$2</f>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV4" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW4" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX4" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY4" t="s">
         <v>7</v>
@@ -7680,19 +7680,19 @@
       </c>
       <c r="TY4" t="str">
         <f t="shared" ref="TY4:UB10" ca="1" si="29">TY$2</f>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ4" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA4" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB4" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC4" t="s">
         <v>691</v>
@@ -7884,19 +7884,19 @@
       </c>
       <c r="ES5" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET5" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU5" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV5" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW5" t="s">
         <v>7</v>
@@ -7906,19 +7906,19 @@
       </c>
       <c r="GC5" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD5" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE5" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF5" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG5" t="s">
         <v>8</v>
@@ -7928,19 +7928,19 @@
       </c>
       <c r="HM5" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN5" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO5" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP5" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ5" t="s">
         <v>7</v>
@@ -7950,19 +7950,19 @@
       </c>
       <c r="IW5" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX5" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY5" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ5" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA5" t="s">
         <v>7</v>
@@ -7972,19 +7972,19 @@
       </c>
       <c r="KG5" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH5" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI5" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ5" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK5" t="s">
         <v>7</v>
@@ -7994,19 +7994,19 @@
       </c>
       <c r="LQ5" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR5" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS5" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT5" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU5" t="s">
         <v>7</v>
@@ -8016,19 +8016,19 @@
       </c>
       <c r="NA5" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB5" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC5" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND5" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE5" t="s">
         <v>7</v>
@@ -8038,19 +8038,19 @@
       </c>
       <c r="OK5" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL5" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM5" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON5" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO5" t="s">
         <v>7</v>
@@ -8060,19 +8060,19 @@
       </c>
       <c r="PU5" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV5" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW5" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX5" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY5" t="s">
         <v>7</v>
@@ -8121,19 +8121,19 @@
       </c>
       <c r="TY5" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ5" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA5" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB5" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC5" t="s">
         <v>691</v>
@@ -8325,19 +8325,19 @@
       </c>
       <c r="ES6" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET6" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU6" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV6" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW6" t="s">
         <v>7</v>
@@ -8347,19 +8347,19 @@
       </c>
       <c r="GC6" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD6" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE6" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF6" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG6" t="s">
         <v>8</v>
@@ -8369,19 +8369,19 @@
       </c>
       <c r="HM6" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN6" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO6" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP6" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ6" t="s">
         <v>7</v>
@@ -8391,19 +8391,19 @@
       </c>
       <c r="IW6" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX6" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY6" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ6" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA6" t="s">
         <v>7</v>
@@ -8413,19 +8413,19 @@
       </c>
       <c r="KG6" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH6" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI6" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ6" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK6" t="s">
         <v>7</v>
@@ -8435,19 +8435,19 @@
       </c>
       <c r="LQ6" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR6" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS6" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT6" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU6" t="s">
         <v>7</v>
@@ -8457,19 +8457,19 @@
       </c>
       <c r="NA6" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB6" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC6" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND6" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE6" t="s">
         <v>7</v>
@@ -8479,19 +8479,19 @@
       </c>
       <c r="OK6" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL6" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM6" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON6" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO6" t="s">
         <v>7</v>
@@ -8501,19 +8501,19 @@
       </c>
       <c r="PU6" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV6" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW6" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX6" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY6" t="s">
         <v>7</v>
@@ -8562,19 +8562,19 @@
       </c>
       <c r="TY6" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ6" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA6" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB6" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC6" t="s">
         <v>691</v>
@@ -8766,19 +8766,19 @@
       </c>
       <c r="ES7" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET7" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU7" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV7" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW7" t="s">
         <v>7</v>
@@ -8788,19 +8788,19 @@
       </c>
       <c r="GC7" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD7" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE7" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF7" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG7" t="s">
         <v>8</v>
@@ -8810,19 +8810,19 @@
       </c>
       <c r="HM7" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN7" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO7" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP7" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ7" t="s">
         <v>7</v>
@@ -8832,19 +8832,19 @@
       </c>
       <c r="IW7" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX7" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY7" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ7" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA7" t="s">
         <v>7</v>
@@ -8854,19 +8854,19 @@
       </c>
       <c r="KG7" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH7" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI7" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ7" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK7" t="s">
         <v>7</v>
@@ -8876,19 +8876,19 @@
       </c>
       <c r="LQ7" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR7" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS7" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT7" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU7" t="s">
         <v>7</v>
@@ -8898,19 +8898,19 @@
       </c>
       <c r="NA7" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB7" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC7" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND7" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE7" t="s">
         <v>7</v>
@@ -8920,19 +8920,19 @@
       </c>
       <c r="OK7" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL7" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM7" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON7" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO7" t="s">
         <v>7</v>
@@ -8942,19 +8942,19 @@
       </c>
       <c r="PU7" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV7" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW7" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX7" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY7" t="s">
         <v>7</v>
@@ -9003,19 +9003,19 @@
       </c>
       <c r="TY7" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ7" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA7" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB7" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC7" t="s">
         <v>691</v>
@@ -9207,19 +9207,19 @@
       </c>
       <c r="ES8" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET8" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU8" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV8" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW8" t="s">
         <v>7</v>
@@ -9229,19 +9229,19 @@
       </c>
       <c r="GC8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG8" t="s">
         <v>8</v>
@@ -9251,19 +9251,19 @@
       </c>
       <c r="HM8" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN8" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO8" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP8" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ8" t="s">
         <v>7</v>
@@ -9273,19 +9273,19 @@
       </c>
       <c r="IW8" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX8" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY8" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ8" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA8" t="s">
         <v>7</v>
@@ -9295,19 +9295,19 @@
       </c>
       <c r="KG8" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH8" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI8" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ8" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK8" t="s">
         <v>7</v>
@@ -9317,19 +9317,19 @@
       </c>
       <c r="LQ8" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR8" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS8" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT8" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU8" t="s">
         <v>7</v>
@@ -9339,19 +9339,19 @@
       </c>
       <c r="NA8" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB8" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC8" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND8" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE8" t="s">
         <v>7</v>
@@ -9361,19 +9361,19 @@
       </c>
       <c r="OK8" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL8" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM8" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON8" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO8" t="s">
         <v>7</v>
@@ -9383,19 +9383,19 @@
       </c>
       <c r="PU8" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV8" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW8" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX8" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY8" t="s">
         <v>7</v>
@@ -9444,19 +9444,19 @@
       </c>
       <c r="TY8" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ8" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA8" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB8" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC8" t="s">
         <v>691</v>
@@ -9648,19 +9648,19 @@
       </c>
       <c r="ES9" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET9" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU9" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV9" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW9" t="s">
         <v>7</v>
@@ -9670,19 +9670,19 @@
       </c>
       <c r="GC9" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD9" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE9" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF9" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG9" t="s">
         <v>8</v>
@@ -9692,19 +9692,19 @@
       </c>
       <c r="HM9" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN9" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO9" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP9" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ9" t="s">
         <v>7</v>
@@ -9714,19 +9714,19 @@
       </c>
       <c r="IW9" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX9" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY9" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ9" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA9" t="s">
         <v>7</v>
@@ -9736,19 +9736,19 @@
       </c>
       <c r="KG9" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH9" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI9" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ9" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK9" t="s">
         <v>7</v>
@@ -9758,19 +9758,19 @@
       </c>
       <c r="LQ9" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR9" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS9" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT9" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU9" t="s">
         <v>7</v>
@@ -9780,19 +9780,19 @@
       </c>
       <c r="NA9" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB9" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC9" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND9" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE9" t="s">
         <v>7</v>
@@ -9802,19 +9802,19 @@
       </c>
       <c r="OK9" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL9" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM9" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON9" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO9" t="s">
         <v>7</v>
@@ -9824,19 +9824,19 @@
       </c>
       <c r="PU9" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV9" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW9" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX9" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY9" t="s">
         <v>7</v>
@@ -9885,19 +9885,19 @@
       </c>
       <c r="TY9" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ9" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA9" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB9" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC9" t="s">
         <v>691</v>
@@ -10089,19 +10089,19 @@
       </c>
       <c r="ES10" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>pqqx</v>
+        <v>wkbm</v>
       </c>
       <c r="ET10" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>priw</v>
+        <v>edtq</v>
       </c>
       <c r="EU10" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>xdms</v>
+        <v>jwse</v>
       </c>
       <c r="EV10" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>ldsy</v>
+        <v>jttf</v>
       </c>
       <c r="EW10" t="s">
         <v>7</v>
@@ -10111,19 +10111,19 @@
       </c>
       <c r="GC10" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>fais</v>
+        <v>vgwt</v>
       </c>
       <c r="GD10" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>vqis</v>
+        <v>xphz</v>
       </c>
       <c r="GE10" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>jian</v>
+        <v>qchf</v>
       </c>
       <c r="GF10" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>eexl</v>
+        <v>lphg</v>
       </c>
       <c r="GG10" t="s">
         <v>8</v>
@@ -10133,19 +10133,19 @@
       </c>
       <c r="HM10" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>gcsf</v>
+        <v>nosv</v>
       </c>
       <c r="HN10" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>zmez</v>
+        <v>lxvm</v>
       </c>
       <c r="HO10" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>wekj</v>
+        <v>ishd</v>
       </c>
       <c r="HP10" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>ruds</v>
+        <v>pmcw</v>
       </c>
       <c r="HQ10" t="s">
         <v>7</v>
@@ -10155,19 +10155,19 @@
       </c>
       <c r="IW10" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>aciq</v>
+        <v>kwoc</v>
       </c>
       <c r="IX10" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>xbho</v>
+        <v>llut</v>
       </c>
       <c r="IY10" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>fwwc</v>
+        <v>vcee</v>
       </c>
       <c r="IZ10" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>kkcn</v>
+        <v>riqr</v>
       </c>
       <c r="JA10" t="s">
         <v>7</v>
@@ -10177,19 +10177,19 @@
       </c>
       <c r="KG10" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>kwvh</v>
+        <v>cbih</v>
       </c>
       <c r="KH10" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>ckba</v>
+        <v>zjzs</v>
       </c>
       <c r="KI10" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>oaaq</v>
+        <v>rlah</v>
       </c>
       <c r="KJ10" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>pamd</v>
+        <v>wicu</v>
       </c>
       <c r="KK10" t="s">
         <v>7</v>
@@ -10199,19 +10199,19 @@
       </c>
       <c r="LQ10" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>uirj</v>
+        <v>atib</v>
       </c>
       <c r="LR10" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>mzcj</v>
+        <v>vyqk</v>
       </c>
       <c r="LS10" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>djko</v>
+        <v>chen</v>
       </c>
       <c r="LT10" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>yesv</v>
+        <v>sbem</v>
       </c>
       <c r="LU10" t="s">
         <v>7</v>
@@ -10221,19 +10221,19 @@
       </c>
       <c r="NA10" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>qplq</v>
+        <v>dpbj</v>
       </c>
       <c r="NB10" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>pfup</v>
+        <v>sows</v>
       </c>
       <c r="NC10" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>fjet</v>
+        <v>ocjl</v>
       </c>
       <c r="ND10" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>miwa</v>
+        <v>mdaq</v>
       </c>
       <c r="NE10" t="s">
         <v>7</v>
@@ -10243,19 +10243,19 @@
       </c>
       <c r="OK10" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>icxx</v>
+        <v>ixuw</v>
       </c>
       <c r="OL10" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>lyms</v>
+        <v>ukvq</v>
       </c>
       <c r="OM10" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>uqyr</v>
+        <v>akce</v>
       </c>
       <c r="ON10" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>ceop</v>
+        <v>jltx</v>
       </c>
       <c r="OO10" t="s">
         <v>7</v>
@@ -10265,19 +10265,19 @@
       </c>
       <c r="PU10" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>bmwq</v>
+        <v>pimg</v>
       </c>
       <c r="PV10" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>gozg</v>
+        <v>ybzr</v>
       </c>
       <c r="PW10" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>mjpb</v>
+        <v>joie</v>
       </c>
       <c r="PX10" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>wujy</v>
+        <v>fbyq</v>
       </c>
       <c r="PY10" t="s">
         <v>7</v>
@@ -10326,19 +10326,19 @@
       </c>
       <c r="TY10" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>sexv</v>
+        <v>ozzb</v>
       </c>
       <c r="TZ10" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>svyv</v>
+        <v>ghxs</v>
       </c>
       <c r="UA10" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>ztjp</v>
+        <v>gxeu</v>
       </c>
       <c r="UB10" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>bvip</v>
+        <v>tbbd</v>
       </c>
       <c r="UC10" t="s">
         <v>691</v>

</xml_diff>